<commit_message>
Completed MST 2-approximation implementation
</commit_message>
<xml_diff>
--- a/Data/Algorithm Times.xlsx
+++ b/Data/Algorithm Times.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LBJ\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdtynes/Desktop/Academics/Georgia Tech/CSE 6140 - CSE Algorithms/Project/CSE-6140---Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9081D1A8-F7CC-2440-8DFD-6F6E65E8C241}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10080" windowHeight="5460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="13820" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
   <si>
     <t>Instance</t>
   </si>
@@ -84,12 +85,15 @@
   </si>
   <si>
     <t>LS1-GA</t>
+  </si>
+  <si>
+    <t>MST</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -924,21 +928,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="5" max="5" width="9.140625" style="1"/>
-    <col min="6" max="6" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="1"/>
+    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -963,8 +967,14 @@
       <c r="I1" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -992,8 +1002,15 @@
         <f>H2/B2-1</f>
         <v>0</v>
       </c>
+      <c r="J2">
+        <v>2380448</v>
+      </c>
+      <c r="K2" s="1">
+        <f>J2/B2-1</f>
+        <v>0.18798879907454125</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1021,8 +1038,15 @@
         <f t="shared" ref="I3:I14" si="2">H3/B3-1</f>
         <v>3.4341023601166754E-2</v>
       </c>
+      <c r="J3">
+        <v>10402</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" ref="K3:K14" si="3">J3/B3-1</f>
+        <v>0.37920975868469897</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1050,8 +1074,15 @@
         <f t="shared" si="2"/>
         <v>1.8258917379937678E-2</v>
       </c>
+      <c r="J4">
+        <v>1150963</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="3"/>
+        <v>0.28809919242201776</v>
+      </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1079,8 +1110,15 @@
         <f t="shared" si="2"/>
         <v>6.0786809262389774E-3</v>
       </c>
+      <c r="J5">
+        <v>65712</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>0.2482571282031798</v>
+      </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1108,8 +1146,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="J6">
+        <v>301216</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="3"/>
+        <v>8.3697904674188361E-2</v>
+      </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1137,8 +1182,15 @@
         <f t="shared" si="2"/>
         <v>3.8962073463372882E-2</v>
       </c>
+      <c r="J7">
+        <v>134748</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="3"/>
+        <v>0.34169728470293026</v>
+      </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1166,8 +1218,15 @@
         <f t="shared" si="2"/>
         <v>6.8594780908775244E-2</v>
       </c>
+      <c r="J8">
+        <v>2027107</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="3"/>
+        <v>0.30355548982032854</v>
+      </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1195,8 +1254,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="J9">
+        <v>1646249</v>
+      </c>
+      <c r="K9" s="1">
+        <f t="shared" si="3"/>
+        <v>0.17927751165667738</v>
+      </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1221,11 +1287,18 @@
         <v>1328514</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="2"/>
+        <f>H10/B10-1</f>
         <v>1.0268607713127085</v>
       </c>
+      <c r="J10">
+        <v>838282</v>
+      </c>
+      <c r="K10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.27893338052708505</v>
+      </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1253,8 +1326,15 @@
         <f t="shared" si="2"/>
         <v>0.20399508267135369</v>
       </c>
+      <c r="J11">
+        <v>1134989</v>
+      </c>
+      <c r="K11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.40088200879787106</v>
+      </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1282,8 +1362,15 @@
         <f t="shared" si="2"/>
         <v>0.17287151054583982</v>
       </c>
+      <c r="J12">
+        <v>1675105</v>
+      </c>
+      <c r="K12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.42422614103121115</v>
+      </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1311,8 +1398,15 @@
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
+      <c r="J13">
+        <v>68090</v>
+      </c>
+      <c r="K13" s="1">
+        <f t="shared" si="3"/>
+        <v>8.1445951526317506E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1339,6 +1433,13 @@
       <c r="I14" s="1">
         <f t="shared" si="2"/>
         <v>0.13070703569464026</v>
+      </c>
+      <c r="J14">
+        <v>178249</v>
+      </c>
+      <c r="K14" s="1">
+        <f t="shared" si="3"/>
+        <v>0.34315683186520873</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implemented Random Restarts for SA
New Data Pushed to Table.
</commit_message>
<xml_diff>
--- a/Data/Algorithm Times.xlsx
+++ b/Data/Algorithm Times.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdtynes/Desktop/Academics/Georgia Tech/CSE 6140 - CSE Algorithms/Project/CSE-6140---Project/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\CSE 6140 - Computational Science and Engineering Algorithms\CSE-6140---Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B99E5F1-F60B-FE41-BBD2-3FDD10AA6019}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E14BFFD-FCE1-481B-8F35-E11FB15F9050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12780" yWindow="1420" windowWidth="13820" windowHeight="13680" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19335" yWindow="7110" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>Instance</t>
   </si>
@@ -88,6 +88,18 @@
   </si>
   <si>
     <t>MST</t>
+  </si>
+  <si>
+    <t>LS1-SA-NN-R</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>LS1-SA-NN-R-T</t>
   </si>
 </sst>
 </file>
@@ -230,7 +242,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -408,6 +420,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -571,9 +589,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="10" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -619,7 +643,15 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -929,52 +961,77 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:O18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="K18" sqref="K18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="9.1640625" style="1"/>
-    <col min="6" max="6" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="8" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
+    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" s="5"/>
+      <c r="D1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="M1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="N1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="O1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -995,22 +1052,36 @@
         <f>F2/B2-1</f>
         <v>0</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>2003763</v>
       </c>
       <c r="I2" s="1">
         <f>H2/B2-1</f>
         <v>0</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
+        <v>2003763</v>
+      </c>
+      <c r="K2" s="1">
+        <f t="shared" ref="K2:K5" si="0">J2/$B2-1</f>
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>2003763</v>
+      </c>
+      <c r="M2" s="1">
+        <f>L2/B2-1</f>
+        <v>0</v>
+      </c>
+      <c r="N2">
         <v>2380448</v>
       </c>
-      <c r="K2" s="1">
-        <f>J2/B2-1</f>
+      <c r="O2" s="1">
+        <f>N2/B2-1</f>
         <v>0.18798879907454125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1021,32 +1092,46 @@
         <v>8295</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E14" si="0">D3/B3-1</f>
+        <f t="shared" ref="E3:E14" si="1">D3/B3-1</f>
         <v>9.9840891010342103E-2</v>
       </c>
       <c r="F3">
         <v>8166</v>
       </c>
       <c r="G3" s="1">
-        <f t="shared" ref="G3:G14" si="1">F3/B3-1</f>
+        <f>F3/B3-1</f>
         <v>8.2736674622116091E-2</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="2">
+        <v>8013</v>
+      </c>
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:K14" si="2">H3/B3-1</f>
+        <v>6.2450278440731921E-2</v>
+      </c>
+      <c r="J3" s="2">
+        <v>7763</v>
+      </c>
+      <c r="K3" s="1">
+        <f t="shared" si="0"/>
+        <v>2.9302572261999504E-2</v>
+      </c>
+      <c r="L3">
         <v>7801</v>
       </c>
-      <c r="I3" s="1">
-        <f t="shared" ref="I3:I14" si="2">H3/B3-1</f>
+      <c r="M3" s="1">
+        <f>L3/B3-1</f>
         <v>3.4341023601166754E-2</v>
       </c>
-      <c r="J3">
+      <c r="N3">
         <v>10402</v>
       </c>
-      <c r="K3" s="1">
-        <f t="shared" ref="K3:K14" si="3">J3/B3-1</f>
+      <c r="O3" s="1">
+        <f>N3/B3-1</f>
         <v>0.37920975868469897</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1057,32 +1142,46 @@
         <v>926357</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.6731592235791366E-2</v>
       </c>
       <c r="F4">
         <v>942768</v>
       </c>
       <c r="G4" s="1">
-        <f t="shared" si="1"/>
+        <f>F4/B4-1</f>
         <v>5.5097947928231195E-2</v>
       </c>
-      <c r="H4">
-        <v>909851</v>
+      <c r="H4" s="2">
+        <v>899396</v>
       </c>
       <c r="I4" s="1">
         <f t="shared" si="2"/>
+        <v>6.5582136589907858E-3</v>
+      </c>
+      <c r="J4" s="2">
+        <v>898259</v>
+      </c>
+      <c r="K4" s="1">
+        <f t="shared" si="0"/>
+        <v>5.2857411452924552E-3</v>
+      </c>
+      <c r="L4">
+        <v>909851</v>
+      </c>
+      <c r="M4" s="1">
+        <f>L4/B4-1</f>
         <v>1.8258917379937678E-2</v>
       </c>
-      <c r="J4">
+      <c r="N4">
         <v>1150963</v>
       </c>
-      <c r="K4" s="1">
-        <f t="shared" si="3"/>
+      <c r="O4" s="1">
+        <f>N4/B4-1</f>
         <v>0.28809919242201776</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1093,32 +1192,46 @@
         <v>54286</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3.1210227380658484E-2</v>
       </c>
       <c r="F5">
         <v>53200</v>
       </c>
       <c r="G5" s="1">
-        <f t="shared" si="1"/>
+        <f>F5/B5-1</f>
         <v>1.0580703987234763E-2</v>
       </c>
-      <c r="H5">
-        <v>52963</v>
+      <c r="H5" s="2">
+        <v>53200</v>
       </c>
       <c r="I5" s="1">
         <f t="shared" si="2"/>
+        <v>1.0580703987234763E-2</v>
+      </c>
+      <c r="J5" s="2">
+        <v>53200</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="0"/>
+        <v>1.0580703987234763E-2</v>
+      </c>
+      <c r="L5">
+        <v>52963</v>
+      </c>
+      <c r="M5" s="1">
+        <f>L5/B5-1</f>
         <v>6.0786809262389774E-3</v>
       </c>
-      <c r="J5">
+      <c r="N5">
         <v>65712</v>
       </c>
-      <c r="K5" s="1">
-        <f t="shared" si="3"/>
+      <c r="O5" s="1">
+        <f>N5/B5-1</f>
         <v>0.2482571282031798</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1129,32 +1242,46 @@
         <v>277952</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F6">
         <v>277952</v>
       </c>
       <c r="G6" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6">
+        <f>F6/B6-1</f>
+        <v>0</v>
+      </c>
+      <c r="H6" s="2">
         <v>277952</v>
       </c>
       <c r="I6" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J6">
+      <c r="J6" s="2">
+        <v>277952</v>
+      </c>
+      <c r="K6" s="1">
+        <f>J6/$B6-1</f>
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>277952</v>
+      </c>
+      <c r="M6" s="1">
+        <f>L6/B6-1</f>
+        <v>0</v>
+      </c>
+      <c r="N6">
         <v>301216</v>
       </c>
-      <c r="K6" s="1">
-        <f t="shared" si="3"/>
+      <c r="O6" s="1">
+        <f>N6/B6-1</f>
         <v>8.3697904674188361E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1165,32 +1292,46 @@
         <v>109180</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8.7114536348338767E-2</v>
       </c>
       <c r="F7">
         <v>109424</v>
       </c>
       <c r="G7" s="1">
-        <f t="shared" si="1"/>
+        <f>F7/B7-1</f>
         <v>8.9544065079507407E-2</v>
       </c>
-      <c r="H7">
-        <v>104344</v>
+      <c r="H7" s="2">
+        <v>104751</v>
       </c>
       <c r="I7" s="1">
         <f t="shared" si="2"/>
+        <v>4.3014607043641906E-2</v>
+      </c>
+      <c r="J7" s="2">
+        <v>105342</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" ref="K7:K14" si="3">J7/$B7-1</f>
+        <v>4.889924425725134E-2</v>
+      </c>
+      <c r="L7">
+        <v>104344</v>
+      </c>
+      <c r="M7" s="1">
+        <f>L7/B7-1</f>
         <v>3.8962073463372882E-2</v>
       </c>
-      <c r="J7">
+      <c r="N7">
         <v>134748</v>
       </c>
-      <c r="K7" s="1">
-        <f t="shared" si="3"/>
+      <c r="O7" s="1">
+        <f>N7/B7-1</f>
         <v>0.34169728470293026</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1201,32 +1342,46 @@
         <v>1655309</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6.4466322842848589E-2</v>
       </c>
       <c r="F8">
         <v>1592563</v>
       </c>
       <c r="G8" s="1">
-        <f t="shared" si="1"/>
+        <f>F8/B8-1</f>
         <v>2.4116754337453195E-2</v>
       </c>
-      <c r="H8">
-        <v>1661729</v>
+      <c r="H8" s="2">
+        <v>1592563</v>
       </c>
       <c r="I8" s="1">
         <f t="shared" si="2"/>
-        <v>6.8594780908775244E-2</v>
-      </c>
-      <c r="J8">
-        <v>2027107</v>
+        <v>2.4116754337453195E-2</v>
+      </c>
+      <c r="J8" s="2">
+        <v>1562562</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="3"/>
+        <v>4.8242511542961886E-3</v>
+      </c>
+      <c r="L8">
+        <v>1661729</v>
+      </c>
+      <c r="M8" s="1">
+        <f>L8/B8-1</f>
+        <v>6.8594780908775244E-2</v>
+      </c>
+      <c r="N8">
+        <v>2027107</v>
+      </c>
+      <c r="O8" s="1">
+        <f>N8/B8-1</f>
         <v>0.30355548982032854</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1237,32 +1392,46 @@
         <v>1404333</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5.9828894519338149E-3</v>
       </c>
       <c r="F9">
         <v>1404001</v>
       </c>
       <c r="G9" s="1">
-        <f t="shared" si="1"/>
+        <f>F9/B9-1</f>
         <v>5.7450638654823472E-3</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="2">
         <v>1395981</v>
       </c>
       <c r="I9" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J9">
-        <v>1646249</v>
+      <c r="J9" s="2">
+        <v>1395981</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>1395981</v>
+      </c>
+      <c r="M9" s="1">
+        <f>L9/B9-1</f>
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1646249</v>
+      </c>
+      <c r="O9" s="1">
+        <f>N9/B9-1</f>
         <v>0.17927751165667738</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1273,32 +1442,46 @@
         <v>1076717</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.64270414094658057</v>
       </c>
       <c r="F10">
         <v>773359</v>
       </c>
       <c r="G10" s="1">
-        <f t="shared" si="1"/>
+        <f>F10/B10-1</f>
         <v>0.17988295135890553</v>
       </c>
-      <c r="H10">
-        <v>1328514</v>
+      <c r="H10" s="2">
+        <v>773359</v>
       </c>
       <c r="I10" s="1">
-        <f>H10/B10-1</f>
-        <v>1.0268607713127085</v>
-      </c>
-      <c r="J10">
-        <v>838282</v>
+        <f t="shared" si="2"/>
+        <v>0.17988295135890553</v>
+      </c>
+      <c r="J10" s="2">
+        <v>773359</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" si="3"/>
+        <v>0.17988295135890553</v>
+      </c>
+      <c r="L10">
+        <v>1328514</v>
+      </c>
+      <c r="M10" s="1">
+        <f>L10/B10-1</f>
+        <v>1.0268607713127085</v>
+      </c>
+      <c r="N10">
+        <v>838282</v>
+      </c>
+      <c r="O10" s="1">
+        <f>N10/B10-1</f>
         <v>0.27893338052708505</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1309,32 +1492,46 @@
         <v>874090</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7.8862398728208882E-2</v>
       </c>
       <c r="F11">
         <v>893034</v>
       </c>
       <c r="G11" s="1">
-        <f t="shared" si="1"/>
+        <f>F11/B11-1</f>
         <v>0.10224439518338779</v>
       </c>
-      <c r="H11">
-        <v>975472</v>
+      <c r="H11" s="2">
+        <v>872737</v>
       </c>
       <c r="I11" s="1">
         <f t="shared" si="2"/>
-        <v>0.20399508267135369</v>
-      </c>
-      <c r="J11">
-        <v>1134989</v>
+        <v>7.7192432448444537E-2</v>
+      </c>
+      <c r="J11" s="2">
+        <v>829710</v>
       </c>
       <c r="K11" s="1">
         <f t="shared" si="3"/>
+        <v>2.4085529921154869E-2</v>
+      </c>
+      <c r="L11">
+        <v>975472</v>
+      </c>
+      <c r="M11" s="1">
+        <f>L11/B11-1</f>
+        <v>0.20399508267135369</v>
+      </c>
+      <c r="N11">
+        <v>1134989</v>
+      </c>
+      <c r="O11" s="1">
+        <f>N11/B11-1</f>
         <v>0.40088200879787106</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1345,32 +1542,46 @@
         <v>1324511</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.12614026600325978</v>
       </c>
       <c r="F12">
         <v>1328318</v>
       </c>
       <c r="G12" s="1">
-        <f t="shared" si="1"/>
+        <f>F12/B12-1</f>
         <v>0.12937709528793495</v>
       </c>
-      <c r="H12">
-        <v>1379474</v>
+      <c r="H12" s="2">
+        <v>1266114</v>
       </c>
       <c r="I12" s="1">
         <f t="shared" si="2"/>
-        <v>0.17287151054583982</v>
-      </c>
-      <c r="J12">
-        <v>1675105</v>
+        <v>7.6489328326039718E-2</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1240675</v>
       </c>
       <c r="K12" s="1">
         <f t="shared" si="3"/>
+        <v>5.4860302801255978E-2</v>
+      </c>
+      <c r="L12">
+        <v>1379474</v>
+      </c>
+      <c r="M12" s="1">
+        <f>L12/B12-1</f>
+        <v>0.17287151054583982</v>
+      </c>
+      <c r="N12">
+        <v>1675105</v>
+      </c>
+      <c r="O12" s="1">
+        <f>N12/B12-1</f>
         <v>0.42422614103121115</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1381,32 +1592,46 @@
         <v>62962</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="F13">
         <v>62962</v>
       </c>
       <c r="G13" s="1">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H13">
+        <f>F13/B13-1</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="2">
         <v>62962</v>
       </c>
       <c r="I13" s="1">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="J13">
-        <v>68090</v>
+      <c r="J13" s="2">
+        <v>62962</v>
       </c>
       <c r="K13" s="1">
         <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>62962</v>
+      </c>
+      <c r="M13" s="1">
+        <f>L13/B13-1</f>
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>68090</v>
+      </c>
+      <c r="O13" s="1">
+        <f>N13/B13-1</f>
         <v>8.1445951526317506E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1417,32 +1642,109 @@
         <v>151072</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>0.13837041948925854</v>
       </c>
       <c r="F14">
         <v>146670</v>
       </c>
       <c r="G14" s="1">
-        <f t="shared" si="1"/>
+        <f>F14/B14-1</f>
         <v>0.10520009946574826</v>
       </c>
-      <c r="H14">
-        <v>150055</v>
+      <c r="H14" s="2">
+        <v>141490</v>
       </c>
       <c r="I14" s="1">
         <f t="shared" si="2"/>
-        <v>0.13070703569464026</v>
-      </c>
-      <c r="J14">
-        <v>178249</v>
+        <v>6.6167328515775115E-2</v>
+      </c>
+      <c r="J14" s="2">
+        <v>138286</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="3"/>
+        <v>4.2024278684942296E-2</v>
+      </c>
+      <c r="L14">
+        <v>150055</v>
+      </c>
+      <c r="M14" s="1">
+        <f>L14/B14-1</f>
+        <v>0.13070703569464026</v>
+      </c>
+      <c r="N14">
+        <v>178249</v>
+      </c>
+      <c r="O14" s="1">
+        <f>N14/B14-1</f>
         <v>0.34315683186520873</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1">
+        <f>AVERAGE(E2:E14)</f>
+        <v>0.1008787449567093</v>
+      </c>
+      <c r="G17" s="1">
+        <f>AVERAGE(G2:G14)</f>
+        <v>6.0348134701230891E-2</v>
+      </c>
+      <c r="I17" s="1">
+        <f>AVERAGE(I2:I14)</f>
+        <v>4.2034815239785958E-2</v>
+      </c>
+      <c r="K17" s="1">
+        <f>AVERAGE(K2:K14)</f>
+        <v>3.0749659659410226E-2</v>
+      </c>
+      <c r="M17" s="1">
+        <f>AVERAGE(M2:M14)</f>
+        <v>0.13082075973107951</v>
+      </c>
+      <c r="O17" s="1">
+        <f>AVERAGE(O2:O14)</f>
+        <v>0.27234056792201966</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="1">
+        <f>STDEV(E2:E14)</f>
+        <v>0.16983398533490765</v>
+      </c>
+      <c r="G18" s="1">
+        <f>STDEV(G2:G14)</f>
+        <v>5.908925185941824E-2</v>
+      </c>
+      <c r="I18" s="1">
+        <f>STDEV(I2:I14)</f>
+        <v>5.1689876126683333E-2</v>
+      </c>
+      <c r="K18" s="1">
+        <f>STDEV(K2:K14)</f>
+        <v>4.9019198577380886E-2</v>
+      </c>
+      <c r="M18" s="1">
+        <f>STDEV(M2:M14)</f>
+        <v>0.27813604763401295</v>
+      </c>
+      <c r="O18" s="1">
+        <f>STDEV(O2:O14)</f>
+        <v>0.11198489326472565</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D1:O14">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
SA Random restarts upon convergence with time bounds added
</commit_message>
<xml_diff>
--- a/Data/Algorithm Times.xlsx
+++ b/Data/Algorithm Times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\CSE 6140 - Computational Science and Engineering Algorithms\CSE-6140---Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E14BFFD-FCE1-481B-8F35-E11FB15F9050}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0855D755-DC22-49E9-8904-F818D246BEB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19335" yWindow="7110" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12900" yWindow="5460" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Instance</t>
   </si>
@@ -90,16 +90,19 @@
     <t>MST</t>
   </si>
   <si>
-    <t>LS1-SA-NN-R</t>
-  </si>
-  <si>
     <t>Mean</t>
   </si>
   <si>
     <t>Stdev</t>
   </si>
   <si>
-    <t>LS1-SA-NN-R-T</t>
+    <t>LS1-SA-RT</t>
+  </si>
+  <si>
+    <t>LS1-SA-R</t>
+  </si>
+  <si>
+    <t>Time (s)</t>
   </si>
 </sst>
 </file>
@@ -643,7 +646,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -961,10 +971,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O18"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K18" sqref="K18"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,13 +990,14 @@
     <col min="9" max="9" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.85546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="8" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1007,31 +1018,34 @@
         <v>16</v>
       </c>
       <c r="H1" s="7" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>16</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="K1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M1" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1049,7 +1063,7 @@
         <v>2003763</v>
       </c>
       <c r="G2" s="1">
-        <f>F2/B2-1</f>
+        <f t="shared" ref="G2:G14" si="0">F2/B2-1</f>
         <v>0</v>
       </c>
       <c r="H2" s="2">
@@ -1063,25 +1077,28 @@
         <v>2003763</v>
       </c>
       <c r="K2" s="1">
-        <f t="shared" ref="K2:K5" si="0">J2/$B2-1</f>
-        <v>0</v>
-      </c>
-      <c r="L2">
+        <f t="shared" ref="K2:K5" si="1">J2/$B2-1</f>
+        <v>0</v>
+      </c>
+      <c r="L2" s="2">
+        <v>6.8659999999999997</v>
+      </c>
+      <c r="M2">
         <v>2003763</v>
       </c>
-      <c r="M2" s="1">
-        <f>L2/B2-1</f>
-        <v>0</v>
-      </c>
-      <c r="N2">
+      <c r="N2" s="1">
+        <f>M2/B2-1</f>
+        <v>0</v>
+      </c>
+      <c r="O2">
         <v>2380448</v>
       </c>
-      <c r="O2" s="1">
-        <f>N2/B2-1</f>
+      <c r="P2" s="1">
+        <f>O2/B2-1</f>
         <v>0.18798879907454125</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1092,46 +1109,49 @@
         <v>8295</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E14" si="1">D3/B3-1</f>
+        <f t="shared" ref="E3:E14" si="2">D3/B3-1</f>
         <v>9.9840891010342103E-2</v>
       </c>
       <c r="F3">
         <v>8166</v>
       </c>
       <c r="G3" s="1">
-        <f>F3/B3-1</f>
+        <f t="shared" si="0"/>
         <v>8.2736674622116091E-2</v>
       </c>
       <c r="H3" s="2">
         <v>8013</v>
       </c>
       <c r="I3" s="1">
-        <f t="shared" ref="I3:K14" si="2">H3/B3-1</f>
+        <f t="shared" ref="I3:I14" si="3">H3/B3-1</f>
         <v>6.2450278440731921E-2</v>
       </c>
       <c r="J3" s="2">
-        <v>7763</v>
+        <v>7542</v>
       </c>
       <c r="K3" s="1">
-        <f t="shared" si="0"/>
-        <v>2.9302572261999504E-2</v>
-      </c>
-      <c r="L3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L3" s="2">
+        <v>200.566</v>
+      </c>
+      <c r="M3">
         <v>7801</v>
       </c>
-      <c r="M3" s="1">
-        <f>L3/B3-1</f>
+      <c r="N3" s="1">
+        <f>M3/B3-1</f>
         <v>3.4341023601166754E-2</v>
       </c>
-      <c r="N3">
+      <c r="O3">
         <v>10402</v>
       </c>
-      <c r="O3" s="1">
-        <f>N3/B3-1</f>
+      <c r="P3" s="1">
+        <f>O3/B3-1</f>
         <v>0.37920975868469897</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1142,46 +1162,49 @@
         <v>926357</v>
       </c>
       <c r="E4" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.6731592235791366E-2</v>
       </c>
       <c r="F4">
         <v>942768</v>
       </c>
       <c r="G4" s="1">
-        <f>F4/B4-1</f>
+        <f t="shared" si="0"/>
         <v>5.5097947928231195E-2</v>
       </c>
       <c r="H4" s="2">
         <v>899396</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5582136589907858E-3</v>
       </c>
-      <c r="J4" s="2">
-        <v>898259</v>
+      <c r="J4">
+        <v>893536</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" si="0"/>
-        <v>5.2857411452924552E-3</v>
-      </c>
-      <c r="L4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="L4" s="2">
+        <v>292.73200000000003</v>
+      </c>
+      <c r="M4">
         <v>909851</v>
       </c>
-      <c r="M4" s="1">
-        <f>L4/B4-1</f>
+      <c r="N4" s="1">
+        <f>M4/B4-1</f>
         <v>1.8258917379937678E-2</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <v>1150963</v>
       </c>
-      <c r="O4" s="1">
-        <f>N4/B4-1</f>
+      <c r="P4" s="1">
+        <f>O4/B4-1</f>
         <v>0.28809919242201776</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1192,46 +1215,49 @@
         <v>54286</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>3.1210227380658484E-2</v>
       </c>
       <c r="F5">
         <v>53200</v>
       </c>
       <c r="G5" s="1">
-        <f>F5/B5-1</f>
+        <f t="shared" si="0"/>
         <v>1.0580703987234763E-2</v>
       </c>
       <c r="H5" s="2">
         <v>53200</v>
       </c>
       <c r="I5" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.0580703987234763E-2</v>
       </c>
       <c r="J5" s="2">
-        <v>53200</v>
+        <v>52965</v>
       </c>
       <c r="K5" s="1">
-        <f t="shared" si="0"/>
-        <v>1.0580703987234763E-2</v>
-      </c>
-      <c r="L5">
+        <f t="shared" si="1"/>
+        <v>6.1166726820280903E-3</v>
+      </c>
+      <c r="L5" s="2">
+        <v>597.47799999999995</v>
+      </c>
+      <c r="M5">
         <v>52963</v>
       </c>
-      <c r="M5" s="1">
-        <f>L5/B5-1</f>
+      <c r="N5" s="1">
+        <f>M5/B5-1</f>
         <v>6.0786809262389774E-3</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <v>65712</v>
       </c>
-      <c r="O5" s="1">
-        <f>N5/B5-1</f>
+      <c r="P5" s="1">
+        <f>O5/B5-1</f>
         <v>0.2482571282031798</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1242,21 +1268,21 @@
         <v>277952</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F6">
         <v>277952</v>
       </c>
       <c r="G6" s="1">
-        <f>F6/B6-1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H6" s="2">
         <v>277952</v>
       </c>
       <c r="I6" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J6" s="2">
@@ -1266,22 +1292,25 @@
         <f>J6/$B6-1</f>
         <v>0</v>
       </c>
-      <c r="L6">
+      <c r="L6" s="2">
+        <v>3.3180000000000001</v>
+      </c>
+      <c r="M6">
         <v>277952</v>
       </c>
-      <c r="M6" s="1">
-        <f>L6/B6-1</f>
-        <v>0</v>
-      </c>
-      <c r="N6">
+      <c r="N6" s="1">
+        <f>M6/B6-1</f>
+        <v>0</v>
+      </c>
+      <c r="O6">
         <v>301216</v>
       </c>
-      <c r="O6" s="1">
-        <f>N6/B6-1</f>
+      <c r="P6" s="1">
+        <f>O6/B6-1</f>
         <v>8.3697904674188361E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1292,46 +1321,49 @@
         <v>109180</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>8.7114536348338767E-2</v>
       </c>
       <c r="F7">
         <v>109424</v>
       </c>
       <c r="G7" s="1">
-        <f>F7/B7-1</f>
+        <f t="shared" si="0"/>
         <v>8.9544065079507407E-2</v>
       </c>
       <c r="H7" s="2">
         <v>104751</v>
       </c>
       <c r="I7" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>4.3014607043641906E-2</v>
       </c>
       <c r="J7" s="2">
-        <v>105342</v>
+        <v>103391</v>
       </c>
       <c r="K7" s="1">
-        <f t="shared" ref="K7:K14" si="3">J7/$B7-1</f>
-        <v>4.889924425725134E-2</v>
-      </c>
-      <c r="L7">
+        <f t="shared" ref="K7:K14" si="4">J7/$B7-1</f>
+        <v>2.9472971492865652E-2</v>
+      </c>
+      <c r="L7" s="2">
+        <v>596.34</v>
+      </c>
+      <c r="M7">
         <v>104344</v>
       </c>
-      <c r="M7" s="1">
-        <f>L7/B7-1</f>
+      <c r="N7" s="1">
+        <f>M7/B7-1</f>
         <v>3.8962073463372882E-2</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <v>134748</v>
       </c>
-      <c r="O7" s="1">
-        <f>N7/B7-1</f>
+      <c r="P7" s="1">
+        <f>O7/B7-1</f>
         <v>0.34169728470293026</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1342,46 +1374,46 @@
         <v>1655309</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>6.4466322842848589E-2</v>
       </c>
       <c r="F8">
         <v>1592563</v>
       </c>
       <c r="G8" s="1">
-        <f>F8/B8-1</f>
+        <f t="shared" si="0"/>
         <v>2.4116754337453195E-2</v>
       </c>
       <c r="H8" s="2">
         <v>1592563</v>
       </c>
       <c r="I8" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.4116754337453195E-2</v>
       </c>
       <c r="J8" s="2">
-        <v>1562562</v>
+        <v>1582057</v>
       </c>
       <c r="K8" s="1">
-        <f t="shared" si="3"/>
-        <v>4.8242511542961886E-3</v>
-      </c>
-      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>1.7360744923025528E-2</v>
+      </c>
+      <c r="M8">
         <v>1661729</v>
       </c>
-      <c r="M8" s="1">
-        <f>L8/B8-1</f>
+      <c r="N8" s="1">
+        <f>M8/B8-1</f>
         <v>6.8594780908775244E-2</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <v>2027107</v>
       </c>
-      <c r="O8" s="1">
-        <f>N8/B8-1</f>
+      <c r="P8" s="1">
+        <f>O8/B8-1</f>
         <v>0.30355548982032854</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1392,46 +1424,46 @@
         <v>1404333</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>5.9828894519338149E-3</v>
       </c>
       <c r="F9">
         <v>1404001</v>
       </c>
       <c r="G9" s="1">
-        <f>F9/B9-1</f>
+        <f t="shared" si="0"/>
         <v>5.7450638654823472E-3</v>
       </c>
       <c r="H9" s="2">
         <v>1395981</v>
       </c>
       <c r="I9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J9" s="2">
         <v>1395981</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L9">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
         <v>1395981</v>
       </c>
-      <c r="M9" s="1">
-        <f>L9/B9-1</f>
-        <v>0</v>
-      </c>
-      <c r="N9">
+      <c r="N9" s="1">
+        <f>M9/B9-1</f>
+        <v>0</v>
+      </c>
+      <c r="O9">
         <v>1646249</v>
       </c>
-      <c r="O9" s="1">
-        <f>N9/B9-1</f>
+      <c r="P9" s="1">
+        <f>O9/B9-1</f>
         <v>0.17927751165667738</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1442,46 +1474,46 @@
         <v>1076717</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.64270414094658057</v>
       </c>
       <c r="F10">
         <v>773359</v>
       </c>
       <c r="G10" s="1">
-        <f>F10/B10-1</f>
+        <f t="shared" si="0"/>
         <v>0.17988295135890553</v>
       </c>
       <c r="H10" s="2">
         <v>773359</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.17988295135890553</v>
       </c>
       <c r="J10" s="2">
         <v>773359</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.17988295135890553</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <v>1328514</v>
       </c>
-      <c r="M10" s="1">
-        <f>L10/B10-1</f>
+      <c r="N10" s="1">
+        <f>M10/B10-1</f>
         <v>1.0268607713127085</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <v>838282</v>
       </c>
-      <c r="O10" s="1">
-        <f>N10/B10-1</f>
+      <c r="P10" s="1">
+        <f>O10/B10-1</f>
         <v>0.27893338052708505</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1492,46 +1524,46 @@
         <v>874090</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.8862398728208882E-2</v>
       </c>
       <c r="F11">
         <v>893034</v>
       </c>
       <c r="G11" s="1">
-        <f>F11/B11-1</f>
+        <f t="shared" si="0"/>
         <v>0.10224439518338779</v>
       </c>
       <c r="H11" s="2">
         <v>872737</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.7192432448444537E-2</v>
       </c>
       <c r="J11" s="2">
         <v>829710</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.4085529921154869E-2</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <v>975472</v>
       </c>
-      <c r="M11" s="1">
-        <f>L11/B11-1</f>
+      <c r="N11" s="1">
+        <f>M11/B11-1</f>
         <v>0.20399508267135369</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <v>1134989</v>
       </c>
-      <c r="O11" s="1">
-        <f>N11/B11-1</f>
+      <c r="P11" s="1">
+        <f>O11/B11-1</f>
         <v>0.40088200879787106</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1542,46 +1574,46 @@
         <v>1324511</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.12614026600325978</v>
       </c>
       <c r="F12">
         <v>1328318</v>
       </c>
       <c r="G12" s="1">
-        <f>F12/B12-1</f>
+        <f t="shared" si="0"/>
         <v>0.12937709528793495</v>
       </c>
       <c r="H12" s="2">
         <v>1266114</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.6489328326039718E-2</v>
       </c>
       <c r="J12" s="2">
         <v>1240675</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.4860302801255978E-2</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <v>1379474</v>
       </c>
-      <c r="M12" s="1">
-        <f>L12/B12-1</f>
+      <c r="N12" s="1">
+        <f>M12/B12-1</f>
         <v>0.17287151054583982</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <v>1675105</v>
       </c>
-      <c r="O12" s="1">
-        <f>N12/B12-1</f>
+      <c r="P12" s="1">
+        <f>O12/B12-1</f>
         <v>0.42422614103121115</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1592,46 +1624,46 @@
         <v>62962</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="F13">
         <v>62962</v>
       </c>
       <c r="G13" s="1">
-        <f>F13/B13-1</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="H13" s="2">
         <v>62962</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="J13" s="2">
         <v>62962</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="L13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>62962</v>
       </c>
-      <c r="M13" s="1">
-        <f>L13/B13-1</f>
-        <v>0</v>
-      </c>
-      <c r="N13">
+      <c r="N13" s="1">
+        <f>M13/B13-1</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
         <v>68090</v>
       </c>
-      <c r="O13" s="1">
-        <f>N13/B13-1</f>
+      <c r="P13" s="1">
+        <f>O13/B13-1</f>
         <v>8.1445951526317506E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1642,48 +1674,48 @@
         <v>151072</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.13837041948925854</v>
       </c>
       <c r="F14">
         <v>146670</v>
       </c>
       <c r="G14" s="1">
-        <f>F14/B14-1</f>
+        <f t="shared" si="0"/>
         <v>0.10520009946574826</v>
       </c>
       <c r="H14" s="2">
         <v>141490</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.6167328515775115E-2</v>
       </c>
       <c r="J14" s="2">
         <v>138286</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>4.2024278684942296E-2</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <v>150055</v>
       </c>
-      <c r="M14" s="1">
-        <f>L14/B14-1</f>
+      <c r="N14" s="1">
+        <f>M14/B14-1</f>
         <v>0.13070703569464026</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <v>178249</v>
       </c>
-      <c r="O14" s="1">
-        <f>N14/B14-1</f>
+      <c r="P14" s="1">
+        <f>O14/B14-1</f>
         <v>0.34315683186520873</v>
       </c>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1">
         <f>AVERAGE(E2:E14)</f>
@@ -1699,20 +1731,20 @@
       </c>
       <c r="K17" s="1">
         <f>AVERAGE(K2:K14)</f>
-        <v>3.0749659659410226E-2</v>
-      </c>
-      <c r="M17" s="1">
-        <f>AVERAGE(M2:M14)</f>
+        <v>2.7215650143398305E-2</v>
+      </c>
+      <c r="N17" s="1">
+        <f>AVERAGE(N2:N14)</f>
         <v>0.13082075973107951</v>
       </c>
-      <c r="O17" s="1">
-        <f>AVERAGE(O2:O14)</f>
+      <c r="P17" s="1">
+        <f>AVERAGE(P2:P14)</f>
         <v>0.27234056792201966</v>
       </c>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E18" s="1">
         <f>STDEV(E2:E14)</f>
@@ -1728,20 +1760,49 @@
       </c>
       <c r="K18" s="1">
         <f>STDEV(K2:K14)</f>
-        <v>4.9019198577380886E-2</v>
-      </c>
-      <c r="M18" s="1">
-        <f>STDEV(M2:M14)</f>
+        <v>4.9406608866077631E-2</v>
+      </c>
+      <c r="N18" s="1">
+        <f>STDEV(N2:N14)</f>
         <v>0.27813604763401295</v>
       </c>
-      <c r="O18" s="1">
-        <f>STDEV(O2:O14)</f>
+      <c r="P18" s="1">
+        <f>STDEV(P2:P14)</f>
         <v>0.11198489326472565</v>
       </c>
     </row>
+    <row r="41" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I41">
+        <v>0.9</v>
+      </c>
+    </row>
+    <row r="42" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I42">
+        <f>1-I41</f>
+        <v>9.9999999999999978E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I43">
+        <f>I42/10</f>
+        <v>9.9999999999999985E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I44">
+        <f>1-I43</f>
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="46" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I46">
+        <f>(9+I41)/10</f>
+        <v>0.99</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="D1:O14">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+  <conditionalFormatting sqref="D1:K3 D5:K14 D4:I4 K4 M1:P14">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
SA Data and Experiments
</commit_message>
<xml_diff>
--- a/Data/Algorithm Times.xlsx
+++ b/Data/Algorithm Times.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LBJ\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\CSE 6140 - Computational Science and Engineering Algorithms\CSE-6140---Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63637261-413E-4A9C-9468-C973FE6F8DC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10080" windowHeight="5460"/>
+    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -89,16 +90,16 @@
     <t>Stdev</t>
   </si>
   <si>
-    <t>Time (s)</t>
-  </si>
-  <si>
     <t>LS1-SA-RS</t>
+  </si>
+  <si>
+    <t>Vertices</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -953,25 +954,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="2.140625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="14.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
@@ -981,15 +983,15 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5"/>
-      <c r="D1" s="7" t="s">
+      <c r="C1" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="D1" s="5"/>
+      <c r="E1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>20</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>16</v>
@@ -1011,28 +1013,28 @@
       <c r="B2">
         <v>2003763</v>
       </c>
-      <c r="D2" s="2">
+      <c r="C2">
+        <v>20</v>
+      </c>
+      <c r="E2" s="2">
         <v>2003763</v>
       </c>
-      <c r="E2" s="1">
-        <f t="shared" ref="E2:E5" si="0">D2/$B2-1</f>
+      <c r="F2" s="1">
+        <f t="shared" ref="F2:F5" si="0">E2/$B2-1</f>
         <v>0</v>
-      </c>
-      <c r="F2" s="2">
-        <v>6.8659999999999997</v>
       </c>
       <c r="G2">
         <v>2003763</v>
       </c>
       <c r="H2" s="1">
-        <f t="shared" ref="H2:H14" si="1">G2/B2-1</f>
+        <f>G2/B2-1</f>
         <v>0</v>
       </c>
       <c r="I2">
         <v>2380448</v>
       </c>
       <c r="J2" s="1">
-        <f t="shared" ref="J2:J14" si="2">I2/B2-1</f>
+        <f>I2/B2-1</f>
         <v>0.18798879907454125</v>
       </c>
     </row>
@@ -1043,28 +1045,28 @@
       <c r="B3">
         <v>7542</v>
       </c>
-      <c r="D3" s="2">
+      <c r="C3">
+        <v>52</v>
+      </c>
+      <c r="E3" s="2">
         <v>7542</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F3" s="2">
-        <v>200.566</v>
-      </c>
       <c r="G3">
         <v>7542</v>
       </c>
       <c r="H3" s="1">
-        <f t="shared" si="1"/>
+        <f>G3/B3-1</f>
         <v>0</v>
       </c>
       <c r="I3">
         <v>10402</v>
       </c>
       <c r="J3" s="1">
-        <f t="shared" si="2"/>
+        <f>I3/B3-1</f>
         <v>0.37920975868469897</v>
       </c>
     </row>
@@ -1075,28 +1077,28 @@
       <c r="B4">
         <v>893536</v>
       </c>
-      <c r="D4">
+      <c r="C4">
+        <v>40</v>
+      </c>
+      <c r="E4">
         <v>893536</v>
       </c>
-      <c r="E4" s="1">
+      <c r="F4" s="1">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="F4" s="2">
-        <v>292.73200000000003</v>
-      </c>
       <c r="G4">
         <v>935856</v>
       </c>
       <c r="H4" s="1">
-        <f t="shared" si="1"/>
+        <f>G4/B4-1</f>
         <v>4.736238942807014E-2</v>
       </c>
       <c r="I4">
         <v>1150963</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" si="2"/>
+        <f>I4/B4-1</f>
         <v>0.28809919242201776</v>
       </c>
     </row>
@@ -1107,28 +1109,28 @@
       <c r="B5">
         <v>52643</v>
       </c>
-      <c r="D5" s="2">
-        <v>52965</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="C5">
+        <v>55</v>
+      </c>
+      <c r="E5" s="2">
+        <v>52883</v>
+      </c>
+      <c r="F5" s="1">
         <f t="shared" si="0"/>
-        <v>6.1166726820280903E-3</v>
-      </c>
-      <c r="F5" s="2">
-        <v>597.47799999999995</v>
+        <v>4.5590106946793441E-3</v>
       </c>
       <c r="G5">
         <v>52643</v>
       </c>
       <c r="H5" s="1">
-        <f t="shared" si="1"/>
+        <f>G5/B5-1</f>
         <v>0</v>
       </c>
       <c r="I5">
         <v>65712</v>
       </c>
       <c r="J5" s="1">
-        <f t="shared" si="2"/>
+        <f>I5/B5-1</f>
         <v>0.2482571282031798</v>
       </c>
     </row>
@@ -1139,28 +1141,28 @@
       <c r="B6">
         <v>277952</v>
       </c>
-      <c r="D6" s="2">
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2">
         <v>277952</v>
       </c>
-      <c r="E6" s="1">
-        <f>D6/$B6-1</f>
+      <c r="F6" s="1">
+        <f>E6/$B6-1</f>
         <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>3.3180000000000001</v>
       </c>
       <c r="G6">
         <v>277952</v>
       </c>
       <c r="H6" s="1">
-        <f t="shared" si="1"/>
+        <f>G6/B6-1</f>
         <v>0</v>
       </c>
       <c r="I6">
         <v>301216</v>
       </c>
       <c r="J6" s="1">
-        <f t="shared" si="2"/>
+        <f>I6/B6-1</f>
         <v>8.3697904674188361E-2</v>
       </c>
     </row>
@@ -1171,28 +1173,28 @@
       <c r="B7">
         <v>100431</v>
       </c>
-      <c r="D7" s="2">
+      <c r="C7">
+        <v>83</v>
+      </c>
+      <c r="E7" s="2">
         <v>103391</v>
       </c>
-      <c r="E7" s="1">
-        <f t="shared" ref="E7:E14" si="3">D7/$B7-1</f>
+      <c r="F7" s="1">
+        <f t="shared" ref="F7:F14" si="1">E7/$B7-1</f>
         <v>2.9472971492865652E-2</v>
-      </c>
-      <c r="F7" s="2">
-        <v>596.34</v>
       </c>
       <c r="G7">
         <v>109266</v>
       </c>
       <c r="H7" s="1">
-        <f t="shared" si="1"/>
+        <f>G7/B7-1</f>
         <v>8.7970845655225949E-2</v>
       </c>
       <c r="I7">
         <v>134748</v>
       </c>
       <c r="J7" s="1">
-        <f t="shared" si="2"/>
+        <f>I7/B7-1</f>
         <v>0.34169728470293026</v>
       </c>
     </row>
@@ -1203,28 +1205,28 @@
       <c r="B8">
         <v>1555060</v>
       </c>
-      <c r="D8" s="2">
-        <v>1570015</v>
-      </c>
-      <c r="E8" s="1">
-        <f t="shared" si="3"/>
-        <v>9.6169922703948085E-3</v>
-      </c>
-      <c r="F8" s="2">
-        <v>596.09500000000003</v>
+      <c r="C8">
+        <v>68</v>
+      </c>
+      <c r="E8" s="2">
+        <v>1559530</v>
+      </c>
+      <c r="F8" s="1">
+        <f t="shared" si="1"/>
+        <v>2.8744871580517195E-3</v>
       </c>
       <c r="G8">
         <v>1651384</v>
       </c>
       <c r="H8" s="1">
-        <f t="shared" si="1"/>
+        <f>G8/B8-1</f>
         <v>6.1942304476997778E-2</v>
       </c>
       <c r="I8">
         <v>2027107</v>
       </c>
       <c r="J8" s="1">
-        <f t="shared" si="2"/>
+        <f>I8/B8-1</f>
         <v>0.30355548982032854</v>
       </c>
     </row>
@@ -1235,28 +1237,28 @@
       <c r="B9">
         <v>1395981</v>
       </c>
-      <c r="D9" s="2">
+      <c r="C9">
+        <v>30</v>
+      </c>
+      <c r="E9" s="2">
         <v>1395981</v>
       </c>
-      <c r="E9" s="1">
-        <f t="shared" si="3"/>
+      <c r="F9" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="F9" s="2">
-        <v>22.879000000000001</v>
       </c>
       <c r="G9">
         <v>1400046</v>
       </c>
       <c r="H9" s="1">
-        <f t="shared" si="1"/>
+        <f>G9/B9-1</f>
         <v>2.9119307497738056E-3</v>
       </c>
       <c r="I9">
         <v>1646249</v>
       </c>
       <c r="J9" s="1">
-        <f t="shared" si="2"/>
+        <f>I9/B9-1</f>
         <v>0.17927751165667738</v>
       </c>
     </row>
@@ -1267,28 +1269,28 @@
       <c r="B10">
         <v>655454</v>
       </c>
-      <c r="D10" s="2">
-        <v>771591</v>
-      </c>
-      <c r="E10" s="1">
-        <f>D10/$B10-1</f>
-        <v>0.17718558434306608</v>
-      </c>
-      <c r="F10" s="2">
-        <v>597.40700000000004</v>
+      <c r="C10">
+        <v>230</v>
+      </c>
+      <c r="E10" s="2">
+        <v>871435</v>
+      </c>
+      <c r="F10" s="1">
+        <f>E10/$B10-1</f>
+        <v>0.32951358905430439</v>
       </c>
       <c r="G10">
         <v>747333</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" si="1"/>
+        <f>G10/B10-1</f>
         <v>0.14017612219926945</v>
       </c>
       <c r="I10">
         <v>838282</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" si="2"/>
+        <f>I10/B10-1</f>
         <v>0.27893338052708505</v>
       </c>
     </row>
@@ -1299,28 +1301,28 @@
       <c r="B11">
         <v>810196</v>
       </c>
-      <c r="D11" s="2">
-        <v>834762</v>
-      </c>
-      <c r="E11" s="1">
-        <f t="shared" si="3"/>
-        <v>3.0321058114332722E-2</v>
-      </c>
-      <c r="F11" s="2">
-        <v>598.00300000000004</v>
+      <c r="C11">
+        <v>99</v>
+      </c>
+      <c r="E11" s="2">
+        <v>824389</v>
+      </c>
+      <c r="F11" s="1">
+        <f t="shared" si="1"/>
+        <v>1.7517983302805851E-2</v>
       </c>
       <c r="G11">
         <v>842272</v>
       </c>
       <c r="H11" s="1">
-        <f t="shared" si="1"/>
+        <f>G11/B11-1</f>
         <v>3.9590420095878098E-2</v>
       </c>
       <c r="I11">
         <v>1134989</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="2"/>
+        <f>I11/B11-1</f>
         <v>0.40088200879787106</v>
       </c>
     </row>
@@ -1331,28 +1333,28 @@
       <c r="B12">
         <v>1176151</v>
       </c>
-      <c r="D12" s="2">
+      <c r="C12">
+        <v>109</v>
+      </c>
+      <c r="E12" s="2">
         <v>1242802</v>
       </c>
-      <c r="E12" s="1">
-        <f t="shared" si="3"/>
+      <c r="F12" s="1">
+        <f t="shared" si="1"/>
         <v>5.6668744064324983E-2</v>
-      </c>
-      <c r="F12" s="2">
-        <v>599.46500000000003</v>
       </c>
       <c r="G12">
         <v>1208125</v>
       </c>
       <c r="H12" s="1">
-        <f t="shared" si="1"/>
+        <f>G12/B12-1</f>
         <v>2.7185284882638383E-2</v>
       </c>
       <c r="I12">
         <v>1675105</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="2"/>
+        <f>I12/B12-1</f>
         <v>0.42422614103121115</v>
       </c>
     </row>
@@ -1363,28 +1365,28 @@
       <c r="B13">
         <v>62962</v>
       </c>
-      <c r="D13" s="2">
+      <c r="C13">
+        <v>10</v>
+      </c>
+      <c r="E13" s="2">
         <v>62962</v>
       </c>
-      <c r="E13" s="1">
-        <f t="shared" si="3"/>
+      <c r="F13" s="1">
+        <f t="shared" si="1"/>
         <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>3.32</v>
       </c>
       <c r="G13">
         <v>62962</v>
       </c>
       <c r="H13" s="1">
-        <f t="shared" si="1"/>
+        <f>G13/B13-1</f>
         <v>0</v>
       </c>
       <c r="I13">
         <v>68090</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="2"/>
+        <f>I13/B13-1</f>
         <v>8.1445951526317506E-2</v>
       </c>
     </row>
@@ -1395,28 +1397,28 @@
       <c r="B14">
         <v>132709</v>
       </c>
-      <c r="D14" s="2">
+      <c r="C14">
+        <v>106</v>
+      </c>
+      <c r="E14" s="2">
         <v>139651</v>
       </c>
-      <c r="E14" s="1">
-        <f t="shared" si="3"/>
+      <c r="F14" s="1">
+        <f t="shared" si="1"/>
         <v>5.2309941300137996E-2</v>
-      </c>
-      <c r="F14" s="2">
-        <v>598.03700000000003</v>
       </c>
       <c r="G14">
         <v>146393</v>
       </c>
       <c r="H14" s="1">
-        <f t="shared" si="1"/>
+        <f>G14/B14-1</f>
         <v>0.10311282580684056</v>
       </c>
       <c r="I14">
         <v>178249</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="2"/>
+        <f>I14/B14-1</f>
         <v>0.34315683186520873</v>
       </c>
     </row>
@@ -1424,9 +1426,9 @@
       <c r="B17" t="s">
         <v>18</v>
       </c>
-      <c r="E17" s="1">
-        <f>AVERAGE(E2:E14)</f>
-        <v>2.7822458789780794E-2</v>
+      <c r="F17" s="1">
+        <f>AVERAGE(F2:F14)</f>
+        <v>3.7916671312859224E-2</v>
       </c>
       <c r="H17" s="1">
         <f>AVERAGE(H2:H14)</f>
@@ -1441,9 +1443,9 @@
       <c r="B18" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="1">
-        <f>STDEV(E2:E14)</f>
-        <v>4.932643888765257E-2</v>
+      <c r="F18" s="1">
+        <f>STDEV(F2:F14)</f>
+        <v>8.9926684676016916E-2</v>
       </c>
       <c r="H18" s="1">
         <f>STDEV(H2:H14)</f>
@@ -1455,7 +1457,7 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4 G1:J14 D1:E3 D5:E14">
+  <conditionalFormatting sqref="F4 G1:J14 E1:F3 E5:F14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added trace files and finalized SA
</commit_message>
<xml_diff>
--- a/Data/Algorithm Times.xlsx
+++ b/Data/Algorithm Times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github Projects\CSE 6140 - Computational Science and Engineering Algorithms\CSE-6140---Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63637261-413E-4A9C-9468-C973FE6F8DC3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB58FAF9-A36D-40D2-8751-BE864A55E79B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4290" yWindow="4290" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7995" yWindow="2325" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
@@ -958,7 +958,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,14 +1027,14 @@
         <v>2003763</v>
       </c>
       <c r="H2" s="1">
-        <f>G2/B2-1</f>
+        <f t="shared" ref="H2:H14" si="1">G2/B2-1</f>
         <v>0</v>
       </c>
       <c r="I2">
         <v>2380448</v>
       </c>
       <c r="J2" s="1">
-        <f>I2/B2-1</f>
+        <f t="shared" ref="J2:J14" si="2">I2/B2-1</f>
         <v>0.18798879907454125</v>
       </c>
     </row>
@@ -1059,14 +1059,14 @@
         <v>7542</v>
       </c>
       <c r="H3" s="1">
-        <f>G3/B3-1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I3">
         <v>10402</v>
       </c>
       <c r="J3" s="1">
-        <f>I3/B3-1</f>
+        <f t="shared" si="2"/>
         <v>0.37920975868469897</v>
       </c>
     </row>
@@ -1091,14 +1091,14 @@
         <v>935856</v>
       </c>
       <c r="H4" s="1">
-        <f>G4/B4-1</f>
+        <f t="shared" si="1"/>
         <v>4.736238942807014E-2</v>
       </c>
       <c r="I4">
         <v>1150963</v>
       </c>
       <c r="J4" s="1">
-        <f>I4/B4-1</f>
+        <f t="shared" si="2"/>
         <v>0.28809919242201776</v>
       </c>
     </row>
@@ -1123,14 +1123,14 @@
         <v>52643</v>
       </c>
       <c r="H5" s="1">
-        <f>G5/B5-1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I5">
         <v>65712</v>
       </c>
       <c r="J5" s="1">
-        <f>I5/B5-1</f>
+        <f t="shared" si="2"/>
         <v>0.2482571282031798</v>
       </c>
     </row>
@@ -1155,14 +1155,14 @@
         <v>277952</v>
       </c>
       <c r="H6" s="1">
-        <f>G6/B6-1</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6">
         <v>301216</v>
       </c>
       <c r="J6" s="1">
-        <f>I6/B6-1</f>
+        <f t="shared" si="2"/>
         <v>8.3697904674188361E-2</v>
       </c>
     </row>
@@ -1180,21 +1180,21 @@
         <v>103391</v>
       </c>
       <c r="F7" s="1">
-        <f t="shared" ref="F7:F14" si="1">E7/$B7-1</f>
+        <f t="shared" ref="F7:F14" si="3">E7/$B7-1</f>
         <v>2.9472971492865652E-2</v>
       </c>
       <c r="G7">
         <v>109266</v>
       </c>
       <c r="H7" s="1">
-        <f>G7/B7-1</f>
+        <f t="shared" si="1"/>
         <v>8.7970845655225949E-2</v>
       </c>
       <c r="I7">
         <v>134748</v>
       </c>
       <c r="J7" s="1">
-        <f>I7/B7-1</f>
+        <f t="shared" si="2"/>
         <v>0.34169728470293026</v>
       </c>
     </row>
@@ -1212,21 +1212,21 @@
         <v>1559530</v>
       </c>
       <c r="F8" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>2.8744871580517195E-3</v>
       </c>
       <c r="G8">
         <v>1651384</v>
       </c>
       <c r="H8" s="1">
-        <f>G8/B8-1</f>
+        <f t="shared" si="1"/>
         <v>6.1942304476997778E-2</v>
       </c>
       <c r="I8">
         <v>2027107</v>
       </c>
       <c r="J8" s="1">
-        <f>I8/B8-1</f>
+        <f t="shared" si="2"/>
         <v>0.30355548982032854</v>
       </c>
     </row>
@@ -1244,21 +1244,21 @@
         <v>1395981</v>
       </c>
       <c r="F9" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="G9">
         <v>1400046</v>
       </c>
       <c r="H9" s="1">
-        <f>G9/B9-1</f>
+        <f t="shared" si="1"/>
         <v>2.9119307497738056E-3</v>
       </c>
       <c r="I9">
         <v>1646249</v>
       </c>
       <c r="J9" s="1">
-        <f>I9/B9-1</f>
+        <f t="shared" si="2"/>
         <v>0.17927751165667738</v>
       </c>
     </row>
@@ -1283,14 +1283,14 @@
         <v>747333</v>
       </c>
       <c r="H10" s="1">
-        <f>G10/B10-1</f>
+        <f t="shared" si="1"/>
         <v>0.14017612219926945</v>
       </c>
       <c r="I10">
         <v>838282</v>
       </c>
       <c r="J10" s="1">
-        <f>I10/B10-1</f>
+        <f t="shared" si="2"/>
         <v>0.27893338052708505</v>
       </c>
     </row>
@@ -1308,21 +1308,21 @@
         <v>824389</v>
       </c>
       <c r="F11" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>1.7517983302805851E-2</v>
       </c>
       <c r="G11">
         <v>842272</v>
       </c>
       <c r="H11" s="1">
-        <f>G11/B11-1</f>
+        <f t="shared" si="1"/>
         <v>3.9590420095878098E-2</v>
       </c>
       <c r="I11">
         <v>1134989</v>
       </c>
       <c r="J11" s="1">
-        <f>I11/B11-1</f>
+        <f t="shared" si="2"/>
         <v>0.40088200879787106</v>
       </c>
     </row>
@@ -1337,24 +1337,24 @@
         <v>109</v>
       </c>
       <c r="E12" s="2">
-        <v>1242802</v>
+        <v>1220743</v>
       </c>
       <c r="F12" s="1">
-        <f t="shared" si="1"/>
-        <v>5.6668744064324983E-2</v>
+        <f t="shared" si="3"/>
+        <v>3.7913499202058221E-2</v>
       </c>
       <c r="G12">
         <v>1208125</v>
       </c>
       <c r="H12" s="1">
-        <f>G12/B12-1</f>
+        <f t="shared" si="1"/>
         <v>2.7185284882638383E-2</v>
       </c>
       <c r="I12">
         <v>1675105</v>
       </c>
       <c r="J12" s="1">
-        <f>I12/B12-1</f>
+        <f t="shared" si="2"/>
         <v>0.42422614103121115</v>
       </c>
     </row>
@@ -1372,21 +1372,21 @@
         <v>62962</v>
       </c>
       <c r="F13" s="1">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>62962</v>
+      </c>
+      <c r="H13" s="1">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="G13">
-        <v>62962</v>
-      </c>
-      <c r="H13" s="1">
-        <f>G13/B13-1</f>
-        <v>0</v>
-      </c>
       <c r="I13">
         <v>68090</v>
       </c>
       <c r="J13" s="1">
-        <f>I13/B13-1</f>
+        <f t="shared" si="2"/>
         <v>8.1445951526317506E-2</v>
       </c>
     </row>
@@ -1404,21 +1404,21 @@
         <v>139651</v>
       </c>
       <c r="F14" s="1">
-        <f t="shared" si="1"/>
+        <f t="shared" si="3"/>
         <v>5.2309941300137996E-2</v>
       </c>
       <c r="G14">
         <v>146393</v>
       </c>
       <c r="H14" s="1">
-        <f>G14/B14-1</f>
+        <f t="shared" si="1"/>
         <v>0.10311282580684056</v>
       </c>
       <c r="I14">
         <v>178249</v>
       </c>
       <c r="J14" s="1">
-        <f>I14/B14-1</f>
+        <f t="shared" si="2"/>
         <v>0.34315683186520873</v>
       </c>
     </row>
@@ -1428,7 +1428,7 @@
       </c>
       <c r="F17" s="1">
         <f>AVERAGE(F2:F14)</f>
-        <v>3.7916671312859224E-2</v>
+        <v>3.6473960169607939E-2</v>
       </c>
       <c r="H17" s="1">
         <f>AVERAGE(H2:H14)</f>
@@ -1445,7 +1445,7 @@
       </c>
       <c r="F18" s="1">
         <f>STDEV(F2:F14)</f>
-        <v>8.9926684676016916E-2</v>
+        <v>8.9751046780648616E-2</v>
       </c>
       <c r="H18" s="1">
         <f>STDEV(H2:H14)</f>

</xml_diff>

<commit_message>
Worked on MST algorithm, generated solution files, integrated with tsp main
</commit_message>
<xml_diff>
--- a/Data/Algorithm Times.xlsx
+++ b/Data/Algorithm Times.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LBJ\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdtynes/Desktop/Academics/Georgia Tech/CSE 6140 - CSE Algorithms/Project/CSE-6140---Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3101AFCE-3B86-1749-9548-BF7D67440DFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10080" windowHeight="5460"/>
+    <workbookView xWindow="16740" yWindow="1460" windowWidth="11620" windowHeight="12620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Instance</t>
   </si>
@@ -93,12 +94,15 @@
   </si>
   <si>
     <t>LS1-SA-RS</t>
+  </si>
+  <si>
+    <t>Time</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -953,28 +957,29 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="2.1640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="2" customWidth="1"/>
     <col min="7" max="7" width="8" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.1640625" customWidth="1"/>
+    <col min="10" max="10" width="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -998,13 +1003,16 @@
         <v>15</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="J1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1029,14 +1037,17 @@
         <v>0</v>
       </c>
       <c r="I2">
+        <v>0.01</v>
+      </c>
+      <c r="J2">
         <v>2380448</v>
       </c>
-      <c r="J2" s="1">
-        <f t="shared" ref="J2:J14" si="2">I2/B2-1</f>
+      <c r="K2" s="1">
+        <f t="shared" ref="K2:K14" si="2">J2/B2-1</f>
         <v>0.18798879907454125</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1061,14 +1072,17 @@
         <v>0</v>
       </c>
       <c r="I3">
+        <v>0.224</v>
+      </c>
+      <c r="J3">
         <v>10402</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <f t="shared" si="2"/>
         <v>0.37920975868469897</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1093,14 +1107,17 @@
         <v>4.736238942807014E-2</v>
       </c>
       <c r="I4">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="J4">
         <v>1150963</v>
       </c>
-      <c r="J4" s="1">
+      <c r="K4" s="1">
         <f t="shared" si="2"/>
         <v>0.28809919242201776</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1125,14 +1142,17 @@
         <v>0</v>
       </c>
       <c r="I5">
+        <v>0.249</v>
+      </c>
+      <c r="J5">
         <v>65712</v>
       </c>
-      <c r="J5" s="1">
+      <c r="K5" s="1">
         <f t="shared" si="2"/>
         <v>0.2482571282031798</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1157,14 +1177,17 @@
         <v>0</v>
       </c>
       <c r="I6">
+        <v>2E-3</v>
+      </c>
+      <c r="J6">
         <v>301216</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <f t="shared" si="2"/>
         <v>8.3697904674188361E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1189,14 +1212,17 @@
         <v>8.7970845655225949E-2</v>
       </c>
       <c r="I7">
+        <v>0.79500000000000004</v>
+      </c>
+      <c r="J7">
         <v>134748</v>
       </c>
-      <c r="J7" s="1">
+      <c r="K7" s="1">
         <f t="shared" si="2"/>
         <v>0.34169728470293026</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1221,14 +1247,17 @@
         <v>6.1942304476997778E-2</v>
       </c>
       <c r="I8">
+        <v>0.627</v>
+      </c>
+      <c r="J8">
         <v>2027107</v>
       </c>
-      <c r="J8" s="1">
+      <c r="K8" s="1">
         <f t="shared" si="2"/>
         <v>0.30355548982032854</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1253,14 +1282,17 @@
         <v>2.9119307497738056E-3</v>
       </c>
       <c r="I9">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J9">
         <v>1646249</v>
       </c>
-      <c r="J9" s="1">
+      <c r="K9" s="1">
         <f t="shared" si="2"/>
         <v>0.17927751165667738</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1285,14 +1317,17 @@
         <v>0.14017612219926945</v>
       </c>
       <c r="I10">
-        <v>838282</v>
-      </c>
-      <c r="J10" s="1">
+        <v>42.779000000000003</v>
+      </c>
+      <c r="J10">
+        <v>808235</v>
+      </c>
+      <c r="K10" s="1">
         <f t="shared" si="2"/>
-        <v>0.27893338052708505</v>
+        <v>0.23309187219850669</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1317,14 +1352,17 @@
         <v>3.9590420095878098E-2</v>
       </c>
       <c r="I11">
-        <v>1134989</v>
-      </c>
-      <c r="J11" s="1">
+        <v>1.492</v>
+      </c>
+      <c r="J11">
+        <v>1060717</v>
+      </c>
+      <c r="K11" s="1">
         <f t="shared" si="2"/>
-        <v>0.40088200879787106</v>
+        <v>0.30921036391194234</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1349,14 +1387,17 @@
         <v>2.7185284882638383E-2</v>
       </c>
       <c r="I12">
-        <v>1675105</v>
-      </c>
-      <c r="J12" s="1">
+        <v>3.1469999999999998</v>
+      </c>
+      <c r="J12">
+        <v>1618300</v>
+      </c>
+      <c r="K12" s="1">
         <f t="shared" si="2"/>
-        <v>0.42422614103121115</v>
+        <v>0.37592877105065581</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1381,14 +1422,17 @@
         <v>0</v>
       </c>
       <c r="I13">
-        <v>68090</v>
-      </c>
-      <c r="J13" s="1">
+        <v>2E-3</v>
+      </c>
+      <c r="J13">
+        <v>65561</v>
+      </c>
+      <c r="K13" s="1">
         <f t="shared" si="2"/>
-        <v>8.1445951526317506E-2</v>
+        <v>4.1278866617959986E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1413,14 +1457,17 @@
         <v>0.10311282580684056</v>
       </c>
       <c r="I14">
+        <v>1.8460000000000001</v>
+      </c>
+      <c r="J14">
         <v>178249</v>
       </c>
-      <c r="J14" s="1">
+      <c r="K14" s="1">
         <f t="shared" si="2"/>
         <v>0.34315683186520873</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -1432,12 +1479,13 @@
         <f>AVERAGE(H2:H14)</f>
         <v>3.925016333036109E-2</v>
       </c>
-      <c r="J17" s="1">
-        <f>AVERAGE(J2:J14)</f>
-        <v>0.27234056792201966</v>
+      <c r="I17" s="1"/>
+      <c r="K17" s="1">
+        <f>AVERAGE(K2:K14)</f>
+        <v>0.25495767499098743</v>
       </c>
     </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -1449,13 +1497,14 @@
         <f>STDEV(H2:H14)</f>
         <v>4.6893457274157418E-2</v>
       </c>
-      <c r="J18" s="1">
-        <f>STDEV(J2:J14)</f>
-        <v>0.11198489326472565</v>
+      <c r="I18" s="1"/>
+      <c r="K18" s="1">
+        <f>STDEV(K2:K14)</f>
+        <v>0.10704468295564611</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E4 G1:J14 D1:E3 D5:E14">
+  <conditionalFormatting sqref="E4 D1:E3 D5:E14 G1:K14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Changes made to Algorithm Times excel document
</commit_message>
<xml_diff>
--- a/Data/Algorithm Times.xlsx
+++ b/Data/Algorithm Times.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kdtynes/Desktop/Academics/Georgia Tech/CSE 6140 - CSE Algorithms/Project/CSE-6140---Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3101AFCE-3B86-1749-9548-BF7D67440DFB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26289266-7471-F348-A6D7-2C3D95E0C70C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16740" yWindow="1460" windowWidth="11620" windowHeight="12620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8380" yWindow="1420" windowWidth="15760" windowHeight="12620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="solutions" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Instance</t>
   </si>
@@ -97,6 +97,9 @@
   </si>
   <si>
     <t>Time</t>
+  </si>
+  <si>
+    <t>MST (0 root)</t>
   </si>
 </sst>
 </file>
@@ -640,7 +643,14 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -958,10 +968,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="5" ySplit="13" topLeftCell="G14" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A14" sqref="A14"/>
+      <selection pane="bottomRight" activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -979,7 +992,7 @@
     <col min="11" max="11" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1011,8 +1024,17 @@
       <c r="K1" s="6" t="s">
         <v>15</v>
       </c>
+      <c r="L1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1040,14 +1062,24 @@
         <v>0.01</v>
       </c>
       <c r="J2">
-        <v>2380448</v>
+        <v>2270785</v>
       </c>
       <c r="K2" s="1">
         <f t="shared" ref="K2:K14" si="2">J2/B2-1</f>
+        <v>0.13326027080048886</v>
+      </c>
+      <c r="L2">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="M2">
+        <v>2380448</v>
+      </c>
+      <c r="N2" s="1">
+        <f>M2/B2-1</f>
         <v>0.18798879907454125</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1075,14 +1107,24 @@
         <v>0.224</v>
       </c>
       <c r="J3">
-        <v>10402</v>
+        <v>9550</v>
       </c>
       <c r="K3" s="1">
         <f t="shared" si="2"/>
+        <v>0.26624237602757894</v>
+      </c>
+      <c r="L3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="M3">
+        <v>10402</v>
+      </c>
+      <c r="N3" s="1">
+        <f>M3/B3-1</f>
         <v>0.37920975868469897</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1110,14 +1152,24 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="J4">
-        <v>1150963</v>
+        <v>1028494</v>
       </c>
       <c r="K4" s="1">
         <f t="shared" si="2"/>
+        <v>0.15103812269455297</v>
+      </c>
+      <c r="L4">
+        <v>2E-3</v>
+      </c>
+      <c r="M4">
+        <v>1150963</v>
+      </c>
+      <c r="N4" s="1">
+        <f t="shared" ref="N4:N14" si="3">M4/B4-1</f>
         <v>0.28809919242201776</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1145,14 +1197,24 @@
         <v>0.249</v>
       </c>
       <c r="J5">
-        <v>65712</v>
+        <v>62395</v>
       </c>
       <c r="K5" s="1">
         <f t="shared" si="2"/>
+        <v>0.18524780122713369</v>
+      </c>
+      <c r="L5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="M5">
+        <v>65712</v>
+      </c>
+      <c r="N5" s="1">
+        <f t="shared" si="3"/>
         <v>0.2482571282031798</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1180,14 +1242,24 @@
         <v>2E-3</v>
       </c>
       <c r="J6">
-        <v>301216</v>
+        <v>297490</v>
       </c>
       <c r="K6" s="1">
         <f t="shared" si="2"/>
+        <v>7.0292712410775948E-2</v>
+      </c>
+      <c r="L6">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="M6">
+        <v>301216</v>
+      </c>
+      <c r="N6" s="1">
+        <f t="shared" si="3"/>
         <v>8.3697904674188361E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1198,7 +1270,7 @@
         <v>103391</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ref="E7:E14" si="3">D7/$B7-1</f>
+        <f t="shared" ref="E7:E14" si="4">D7/$B7-1</f>
         <v>2.9472971492865652E-2</v>
       </c>
       <c r="F7" s="2">
@@ -1215,14 +1287,24 @@
         <v>0.79500000000000004</v>
       </c>
       <c r="J7">
-        <v>134748</v>
+        <v>133065</v>
       </c>
       <c r="K7" s="1">
         <f t="shared" si="2"/>
+        <v>0.32493951070884486</v>
+      </c>
+      <c r="L7">
+        <v>1.2E-2</v>
+      </c>
+      <c r="M7">
+        <v>134748</v>
+      </c>
+      <c r="N7" s="1">
+        <f t="shared" si="3"/>
         <v>0.34169728470293026</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1233,7 +1315,7 @@
         <v>1570015</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.6169922703948085E-3</v>
       </c>
       <c r="F8" s="2">
@@ -1250,14 +1332,24 @@
         <v>0.627</v>
       </c>
       <c r="J8">
-        <v>2027107</v>
+        <v>2003747</v>
       </c>
       <c r="K8" s="1">
         <f t="shared" si="2"/>
+        <v>0.28853356140599073</v>
+      </c>
+      <c r="L8">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="M8">
+        <v>2027107</v>
+      </c>
+      <c r="N8" s="1">
+        <f t="shared" si="3"/>
         <v>0.30355548982032854</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1268,7 +1360,7 @@
         <v>1395981</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F9" s="2">
@@ -1285,14 +1377,24 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="J9">
-        <v>1646249</v>
+        <v>1626820</v>
       </c>
       <c r="K9" s="1">
         <f t="shared" si="2"/>
+        <v>0.16535970045437587</v>
+      </c>
+      <c r="L9">
+        <v>2E-3</v>
+      </c>
+      <c r="M9">
+        <v>1646249</v>
+      </c>
+      <c r="N9" s="1">
+        <f t="shared" si="3"/>
         <v>0.17927751165667738</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1326,8 +1428,18 @@
         <f t="shared" si="2"/>
         <v>0.23309187219850669</v>
       </c>
+      <c r="L10">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="M10">
+        <v>838282</v>
+      </c>
+      <c r="N10" s="1">
+        <f t="shared" si="3"/>
+        <v>0.27893338052708505</v>
+      </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
@@ -1338,7 +1450,7 @@
         <v>834762</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3.0321058114332722E-2</v>
       </c>
       <c r="F11" s="2">
@@ -1361,8 +1473,18 @@
         <f t="shared" si="2"/>
         <v>0.30921036391194234</v>
       </c>
+      <c r="L11">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="M11">
+        <v>1134989</v>
+      </c>
+      <c r="N11" s="1">
+        <f t="shared" si="3"/>
+        <v>0.40088200879787106</v>
+      </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
@@ -1373,7 +1495,7 @@
         <v>1242802</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.6668744064324983E-2</v>
       </c>
       <c r="F12" s="2">
@@ -1396,8 +1518,18 @@
         <f t="shared" si="2"/>
         <v>0.37592877105065581</v>
       </c>
+      <c r="L12">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="M12">
+        <v>1675105</v>
+      </c>
+      <c r="N12" s="1">
+        <f t="shared" si="3"/>
+        <v>0.42422614103121115</v>
+      </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1408,7 +1540,7 @@
         <v>62962</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="F13" s="2">
@@ -1431,8 +1563,18 @@
         <f t="shared" si="2"/>
         <v>4.1278866617959986E-2</v>
       </c>
+      <c r="L13">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="M13">
+        <v>68090</v>
+      </c>
+      <c r="N13" s="1">
+        <f t="shared" si="3"/>
+        <v>8.1445951526317506E-2</v>
+      </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
@@ -1443,7 +1585,7 @@
         <v>139651</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.2309941300137996E-2</v>
       </c>
       <c r="F14" s="2">
@@ -1460,14 +1602,24 @@
         <v>1.8460000000000001</v>
       </c>
       <c r="J14">
-        <v>178249</v>
+        <v>165116</v>
       </c>
       <c r="K14" s="1">
         <f t="shared" si="2"/>
+        <v>0.24419594752428253</v>
+      </c>
+      <c r="L14">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="M14">
+        <v>178249</v>
+      </c>
+      <c r="N14" s="1">
+        <f t="shared" si="3"/>
         <v>0.34315683186520873</v>
       </c>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>18</v>
       </c>
@@ -1479,13 +1631,25 @@
         <f>AVERAGE(H2:H14)</f>
         <v>3.925016333036109E-2</v>
       </c>
-      <c r="I17" s="1"/>
+      <c r="I17">
+        <f>AVERAGE(I2:I14)</f>
+        <v>3.9468461538461534</v>
+      </c>
       <c r="K17" s="1">
         <f>AVERAGE(K2:K14)</f>
-        <v>0.25495767499098743</v>
+        <v>0.21450922131023764</v>
+      </c>
+      <c r="L17">
+        <f>AVERAGE(L2:L14)</f>
+        <v>2.2784615384615389E-2</v>
+      </c>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1">
+        <f t="shared" ref="L17:N17" si="5">AVERAGE(N2:N14)</f>
+        <v>0.27234056792201966</v>
       </c>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>19</v>
       </c>
@@ -1497,14 +1661,31 @@
         <f>STDEV(H2:H14)</f>
         <v>4.6893457274157418E-2</v>
       </c>
-      <c r="I18" s="1"/>
+      <c r="I18">
+        <f>STDEV(I3:I15)</f>
+        <v>12.163391142413095</v>
+      </c>
       <c r="K18" s="1">
         <f>STDEV(K2:K14)</f>
-        <v>0.10704468295564611</v>
+        <v>0.10054476646669623</v>
+      </c>
+      <c r="L18">
+        <f>STDEV(L3:L15)</f>
+        <v>5.4761003460491849E-2</v>
+      </c>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1">
+        <f t="shared" ref="L18:N18" si="6">STDEV(N2:N14)</f>
+        <v>0.11198489326472565</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="E4 D1:E3 D5:E14 G1:K14">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:N14">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>